<commit_message>
Added install.packages to script 1
</commit_message>
<xml_diff>
--- a/Results/Tables/Table_c2.xlsx
+++ b/Results/Tables/Table_c2.xlsx
@@ -12,42 +12,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
-    <t>URBAN</t>
+    <t>Var1</t>
   </si>
   <si>
-    <t>INCOME</t>
+    <t>Var2</t>
   </si>
   <si>
-    <t>CASES</t>
+    <t>Freq</t>
   </si>
   <si>
-    <t>Rural</t>
+    <t/>
   </si>
   <si>
-    <t>Urban cluster</t>
+    <t xml:space="preserve">     NO2</t>
   </si>
   <si>
-    <t>Urbanized area</t>
+    <t xml:space="preserve">Min.   : 1.478  </t>
   </si>
   <si>
-    <t>$20,000 to &lt;$35,000</t>
+    <t xml:space="preserve">1st Qu.: 7.941  </t>
   </si>
   <si>
-    <t>$35,000 to &lt;$50,000</t>
+    <t xml:space="preserve">Median :11.385  </t>
   </si>
   <si>
-    <t>$50,000 to &lt;$75,000</t>
+    <t xml:space="preserve">Mean   :13.239  </t>
   </si>
   <si>
-    <t>&lt;$20,000</t>
+    <t xml:space="preserve">3rd Qu.:16.580  </t>
   </si>
   <si>
-    <t>&gt;=$75,000</t>
-  </si>
-  <si>
-    <t>Not defined</t>
+    <t xml:space="preserve">Max.   :58.293  </t>
   </si>
 </sst>
 </file>
@@ -110,113 +107,69 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="e">
-        <v>#N/A</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" t="e">
-        <v>#N/A</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>794933.7984124991</v>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="e">
-        <v>#N/A</v>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
-      <c r="C3" t="n">
-        <v>148470.3366124999</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C4" t="n">
-        <v>75452.78039999995</v>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
-      <c r="B5" t="e">
-        <v>#N/A</v>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
-      <c r="C5" t="n">
-        <v>571010.6814000006</v>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="e">
-        <v>#N/A</v>
+      <c r="A6" t="s">
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
-      <c r="C6" t="n">
-        <v>137765.46886249995</v>
+      <c r="C6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="e">
-        <v>#N/A</v>
+      <c r="A7" t="s">
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
-      <c r="C7" t="n">
-        <v>200366.52877500042</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="n">
-        <v>236827.43735000046</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="n">
-        <v>28207.198149999997</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C7" t="s">
         <v>10</v>
-      </c>
-      <c r="C10" t="n">
-        <v>191620.94071250016</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="n">
-        <v>146.2245625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>